<commit_message>
modified Excel Sheets based on current situation
</commit_message>
<xml_diff>
--- a/PROJECT/BC/BC_EXCEL_SHEETS/Detailed_Estimation_of_Expenditure_Time.xlsx
+++ b/PROJECT/BC/BC_EXCEL_SHEETS/Detailed_Estimation_of_Expenditure_Time.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Adrian Khairi</t>
-  </si>
-  <si>
-    <t>Sophie Kirschner</t>
   </si>
   <si>
     <t>Janin Ahlemeyer</t>
@@ -259,7 +256,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
+              <c:f>Tabelle1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -303,10 +300,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$14</c:f>
+              <c:f>Tabelle1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -361,7 +358,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sophie Kirschner</c:v>
+                  <c:v>Janin Ahlemeyer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -378,7 +375,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
+              <c:f>Tabelle1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -422,33 +419,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$14</c:f>
+              <c:f>Tabelle1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -460,7 +457,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,7 +477,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Janin Ahlemeyer</c:v>
+                  <c:v>Mika Kuge</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -497,7 +494,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
+              <c:f>Tabelle1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -541,39 +538,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$14</c:f>
+              <c:f>Tabelle1!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
@@ -599,7 +596,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mika Kuge</c:v>
+                  <c:v>Maris Koch</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -616,7 +613,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
+              <c:f>Tabelle1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -660,24 +657,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$2:$E$14</c:f>
+              <c:f>Tabelle1!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -686,19 +683,19 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,7 +715,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Maris Koch</c:v>
+                  <c:v>Erika Zhang</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -735,7 +732,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
+              <c:f>Tabelle1!$A$2:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -779,27 +776,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$14</c:f>
+              <c:f>Tabelle1!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
@@ -817,7 +814,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,125 +822,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-212C-4831-B28B-8D22EE1029E9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Erika Zhang</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Protocoling </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Documents</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Product analysis</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Project design</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Coding</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Test </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Meetings</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Customer exchange</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Leading project</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Presentation</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>GitHub</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-212C-4831-B28B-8D22EE1029E9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1354,7 +1232,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sophie Kirschner</c:v>
+                  <c:v>Janin Ahlemeyer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1423,25 +1301,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1453,7 +1331,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,7 +1351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Janin Ahlemeyer</c:v>
+                  <c:v>Mika Kuge</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1542,31 +1420,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
@@ -1592,7 +1470,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mika Kuge</c:v>
+                  <c:v>Maris Koch</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1661,16 +1539,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
@@ -1679,19 +1557,19 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1711,7 +1589,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Maris Koch</c:v>
+                  <c:v>Erika Zhang</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1777,22 +1655,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20</c:v>
@@ -1810,7 +1688,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,125 +1696,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-559A-4E51-8824-219BB68C29B1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Erika Zhang</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Protocoling </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Documents</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Product analysis</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Project design</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Coding</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Test </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Meetings</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Customer exchange</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Leading project</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Presentation</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>GitHub</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-559A-4E51-8824-219BB68C29B1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3291,12 +3050,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G13" totalsRowShown="0" headerRowCellStyle="Standard" dataCellStyle="Standard">
-  <autoFilter ref="A1:G13"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F13" totalsRowShown="0" headerRowCellStyle="Standard" dataCellStyle="Standard">
+  <autoFilter ref="A1:F13"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Tasks" dataCellStyle="Standard"/>
     <tableColumn id="2" name="Adrian Khairi" dataCellStyle="Standard"/>
-    <tableColumn id="3" name="Sophie Kirschner" dataCellStyle="Standard"/>
     <tableColumn id="4" name="Janin Ahlemeyer" dataCellStyle="Standard"/>
     <tableColumn id="5" name="Mika Kuge" dataCellStyle="Standard"/>
     <tableColumn id="6" name="Maris Koch" dataCellStyle="Standard"/>
@@ -3569,26 +3327,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3605,14 +3363,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3627,44 +3382,38 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>40</v>
-      </c>
-      <c r="G3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3673,84 +3422,72 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
         <v>10</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
-      </c>
-      <c r="G6">
-        <v>50</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -3767,36 +3504,30 @@
       <c r="F8">
         <v>20</v>
       </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
       <c r="C9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
         <v>0</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -3813,13 +3544,10 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -3828,21 +3556,18 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
         <v>0</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -3859,34 +3584,28 @@
       <c r="F12">
         <v>10</v>
       </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>15</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F13">
-        <v>25</v>
-      </c>
-      <c r="G13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -3895,7 +3614,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -3907,9 +3626,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"CorpoS"&amp;10&amp;K000000Internal&amp;1#</oddHeader>
-  </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>